<commit_message>
Correccion de observaciones #1
</commit_message>
<xml_diff>
--- a/Web/SPSA.Autorizadores/SPSA.Autorizadores.Web/Plantillas_Tablas/Plantilla_Caja/TablaCaja.xlsx
+++ b/Web/SPSA.Autorizadores/SPSA.Autorizadores.Web/Plantillas_Tablas/Plantilla_Caja/TablaCaja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Experis\Documents\SPSA\Tablas SGP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waly_\source\repos\Spsa\sistema-autorizadores\Web\SPSA.Autorizadores\SPSA.Autorizadores.Web\Plantillas_Tablas\Plantilla_Caja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D41301-125B-470B-BA0A-E2D8409FEB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807FF9A9-BDAB-41DC-839C-ABF28D036559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{19C504CC-7730-483E-972D-57CFE8980AA7}"/>
+    <workbookView xWindow="5016" yWindow="8688" windowWidth="23040" windowHeight="7872" xr2:uid="{19C504CC-7730-483E-972D-57CFE8980AA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
   <si>
     <t>COD_EMPRESA</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>192.168.1.82</t>
+  </si>
+  <si>
+    <t>TIP_UBICACION</t>
+  </si>
+  <si>
+    <t>TIP_CAJA</t>
   </si>
 </sst>
 </file>
@@ -138,9 +144,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -178,7 +184,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -284,7 +290,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -426,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -434,23 +440,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F10B30E3-4C11-4297-A774-1B6A89B2F987}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="5" width="13.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="4" max="5" width="13.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,8 +486,14 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -508,7 +522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -537,7 +551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -566,7 +580,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -595,7 +609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -624,7 +638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -653,7 +667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -802,18 +816,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -833,14 +847,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FD8CCF5-D548-417D-A763-6C909FDA3CA4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F283DB0-D1B7-4E90-955C-7A782166F512}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -853,4 +859,12 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FD8CCF5-D548-417D-A763-6C909FDA3CA4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>